<commit_message>
Added additional results with p-values and sensitivity analyses
</commit_message>
<xml_diff>
--- a/results/mind_aim2-1_gee_AAPC_results_resistance_proportions.xlsx
+++ b/results/mind_aim2-1_gee_AAPC_results_resistance_proportions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm-pham/academia/hsph/mind/data/mind_manuscript_tab_gee_results_Dec2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm-pham/academia/hsph/mind/publications/aim2-1/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170F9302-7FCA-694B-93C2-8636633142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01937AA2-268F-DB4B-8518-18A310E3E1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FQL_class" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,16 @@
     <sheet name="anti_st..." sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'anti_st...'!$B$1:$C$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CPH_03_...'!$B$1:$C$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CPM_class!$B$1:$C$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FQL_class!$B$1:$C$55</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">VANC!$B$1:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CPM_class!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FQL_class!$A$1:$I$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">VANC!$A$1:$I$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="274">
   <si>
     <t>organismofinterest</t>
   </si>
@@ -601,42 +599,6 @@
   </si>
   <si>
     <t>-8.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  7.3% (95%CI: [  0.2,  14.9])</t>
-  </si>
-  <si>
-    <t>7.3*</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11.8% (95%CI: [-24.0,  64.5])</t>
-  </si>
-  <si>
-    <t>11.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  6.7% (95%CI: [ -2.4,  16.8])</t>
-  </si>
-  <si>
-    <t>6.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  7.9% (95%CI: [ -0.6,  17.2])</t>
-  </si>
-  <si>
-    <t>7.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  1.7% (95%CI: [-43.4,  82.8])</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 23.0% (95%CI: [-30.5, 117.5])</t>
-  </si>
-  <si>
-    <t>23</t>
   </si>
   <si>
     <t xml:space="preserve"> -0.1% (95%CI: [ -6.7,   6.9])</t>
@@ -895,16 +857,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -932,9 +886,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,15 +1188,20 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1275,9 +1233,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1286,27 +1244,27 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>-2.6</v>
+        <v>-6.9</v>
       </c>
       <c r="E2">
-        <v>-4.5999999999999996</v>
+        <v>-9.1999999999999993</v>
       </c>
       <c r="F2">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1315,143 +1273,143 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>-11.6</v>
+        <v>22.3</v>
       </c>
       <c r="E3">
-        <v>-19</v>
+        <v>0.8</v>
       </c>
       <c r="F3">
-        <v>-3.6</v>
+        <v>48.3</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>-2.6</v>
+        <v>-6.8</v>
       </c>
       <c r="E4">
-        <v>-4.8</v>
+        <v>-9.5</v>
       </c>
       <c r="F4">
-        <v>-0.5</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5">
-        <v>-2.5</v>
+        <v>21</v>
       </c>
       <c r="E5">
-        <v>-4.7</v>
+        <v>-10.199999999999999</v>
       </c>
       <c r="F5">
-        <v>-0.3</v>
+        <v>62.9</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6">
-        <v>-8.5</v>
+        <v>-6.9</v>
       </c>
       <c r="E6">
-        <v>-16</v>
+        <v>-9.6999999999999993</v>
       </c>
       <c r="F6">
-        <v>-0.3</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>-14.6</v>
+        <v>23.6</v>
       </c>
       <c r="E7">
-        <v>-23.4</v>
+        <v>-0.3</v>
       </c>
       <c r="F7">
-        <v>-4.9000000000000004</v>
+        <v>53.1</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1460,27 +1418,27 @@
         <v>11</v>
       </c>
       <c r="D8">
-        <v>-6.4</v>
+        <v>-6.5</v>
       </c>
       <c r="E8">
         <v>-9.1999999999999993</v>
       </c>
       <c r="F8">
-        <v>-3.6</v>
+        <v>-3.7</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1489,143 +1447,143 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>-9.9</v>
+        <v>12.4</v>
       </c>
       <c r="E9">
-        <v>-20.9</v>
+        <v>-7.2</v>
       </c>
       <c r="F9">
-        <v>2.6</v>
+        <v>36.1</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>-7.1</v>
+        <v>-7.3</v>
       </c>
       <c r="E10">
-        <v>-10.1</v>
+        <v>-10.8</v>
       </c>
       <c r="F10">
-        <v>-4</v>
+        <v>-3.6</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11">
-        <v>-5.7</v>
+        <v>10.6</v>
       </c>
       <c r="E11">
-        <v>-8.5</v>
+        <v>-13.7</v>
       </c>
       <c r="F11">
-        <v>-2.9</v>
+        <v>41.8</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="I11" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>-9.9</v>
+        <v>-5.7</v>
       </c>
       <c r="E12">
-        <v>-21.3</v>
+        <v>-8.9</v>
       </c>
       <c r="F12">
-        <v>3.1</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>-9.9</v>
+        <v>14.1</v>
       </c>
       <c r="E13">
-        <v>-22.4</v>
+        <v>-10.9</v>
       </c>
       <c r="F13">
-        <v>4.5999999999999996</v>
+        <v>46.1</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -1634,27 +1592,27 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <v>-4.5</v>
+        <v>-6.4</v>
       </c>
       <c r="E14">
-        <v>-8.6</v>
+        <v>-9.1999999999999993</v>
       </c>
       <c r="F14">
-        <v>-0.2</v>
+        <v>-3.6</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1663,143 +1621,143 @@
         <v>11</v>
       </c>
       <c r="D15">
-        <v>-4.2</v>
+        <v>-9.9</v>
       </c>
       <c r="E15">
-        <v>-18.2</v>
+        <v>-20.9</v>
       </c>
       <c r="F15">
-        <v>12.1</v>
+        <v>2.6</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16">
-        <v>-4.4000000000000004</v>
+        <v>-5.7</v>
       </c>
       <c r="E16">
-        <v>-8.8000000000000007</v>
+        <v>-8.5</v>
       </c>
       <c r="F16">
-        <v>0.2</v>
+        <v>-2.9</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
       <c r="D17">
-        <v>-4.5999999999999996</v>
+        <v>-9.9</v>
       </c>
       <c r="E17">
-        <v>-8.8000000000000007</v>
+        <v>-22.4</v>
       </c>
       <c r="F17">
-        <v>-0.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I17" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18">
-        <v>-3</v>
+        <v>-7.1</v>
       </c>
       <c r="E18">
-        <v>-19.3</v>
+        <v>-10.1</v>
       </c>
       <c r="F18">
-        <v>16.8</v>
+        <v>-4</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="I18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D19">
-        <v>-5.5</v>
+        <v>-9.9</v>
       </c>
       <c r="E19">
-        <v>-20.7</v>
+        <v>-21.3</v>
       </c>
       <c r="F19">
-        <v>12.6</v>
+        <v>3.1</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="I19" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -1808,27 +1766,27 @@
         <v>11</v>
       </c>
       <c r="D20">
-        <v>-0.1</v>
+        <v>-4.5</v>
       </c>
       <c r="E20">
-        <v>-1.1000000000000001</v>
+        <v>-8.6</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="I20" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -1837,143 +1795,143 @@
         <v>11</v>
       </c>
       <c r="D21">
-        <v>-4.5</v>
+        <v>-4.2</v>
       </c>
       <c r="E21">
-        <v>-8.8000000000000007</v>
+        <v>-18.2</v>
       </c>
       <c r="F21">
-        <v>0.1</v>
+        <v>12.1</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I21" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D22">
-        <v>0.5</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="E22">
-        <v>-0.6</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="F22">
-        <v>1.6</v>
+        <v>-0.2</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23">
-        <v>-0.6</v>
+        <v>-5.5</v>
       </c>
       <c r="E23">
-        <v>-1.8</v>
+        <v>-20.7</v>
       </c>
       <c r="F23">
-        <v>0.6</v>
+        <v>12.6</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24">
-        <v>-4.5</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="E24">
-        <v>-9.6999999999999993</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="F24">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="I24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>-4.4000000000000004</v>
+        <v>-3</v>
       </c>
       <c r="E25">
-        <v>-9.6</v>
+        <v>-19.3</v>
       </c>
       <c r="F25">
-        <v>1.1000000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="I25" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -1982,27 +1940,27 @@
         <v>11</v>
       </c>
       <c r="D26">
-        <v>-1.6</v>
+        <v>-0.1</v>
       </c>
       <c r="E26">
-        <v>-4</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="F26">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="I26" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
@@ -2011,143 +1969,143 @@
         <v>11</v>
       </c>
       <c r="D27">
-        <v>7.6</v>
+        <v>-4.5</v>
       </c>
       <c r="E27">
-        <v>-3.7</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="F27">
-        <v>20.3</v>
+        <v>0.1</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="I27" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28">
-        <v>-0.8</v>
+        <v>-0.6</v>
       </c>
       <c r="E28">
-        <v>-3.3</v>
+        <v>-1.8</v>
       </c>
       <c r="F28">
-        <v>1.7</v>
+        <v>0.6</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="I28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="D29">
-        <v>-2.2999999999999998</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="E29">
-        <v>-5</v>
+        <v>-9.6</v>
       </c>
       <c r="F29">
-        <v>0.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="I29" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30">
-        <v>8.1999999999999993</v>
+        <v>0.5</v>
       </c>
       <c r="E30">
-        <v>-3.4</v>
+        <v>-0.6</v>
       </c>
       <c r="F30">
-        <v>21.1</v>
+        <v>1.6</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="I30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D31">
-        <v>7.1</v>
+        <v>-4.5</v>
       </c>
       <c r="E31">
-        <v>-7.7</v>
+        <v>-9.6999999999999993</v>
       </c>
       <c r="F31">
-        <v>24.3</v>
+        <v>0.9</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="I31" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -2156,27 +2114,27 @@
         <v>11</v>
       </c>
       <c r="D32">
-        <v>-6.5</v>
+        <v>-1.6</v>
       </c>
       <c r="E32">
-        <v>-9.1999999999999993</v>
+        <v>-4</v>
       </c>
       <c r="F32">
-        <v>-3.7</v>
+        <v>0.9</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I32" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
@@ -2185,143 +2143,143 @@
         <v>11</v>
       </c>
       <c r="D33">
-        <v>12.4</v>
+        <v>7.6</v>
       </c>
       <c r="E33">
-        <v>-7.2</v>
+        <v>-3.7</v>
       </c>
       <c r="F33">
-        <v>36.1</v>
+        <v>20.3</v>
       </c>
       <c r="G33" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D34">
-        <v>-5.7</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="E34">
-        <v>-8.9</v>
+        <v>-5</v>
       </c>
       <c r="F34">
-        <v>-2.2999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="G34" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="I34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
         <v>20</v>
       </c>
       <c r="D35">
-        <v>-7.3</v>
+        <v>7.1</v>
       </c>
       <c r="E35">
-        <v>-10.8</v>
+        <v>-7.7</v>
       </c>
       <c r="F35">
-        <v>-3.6</v>
+        <v>24.3</v>
       </c>
       <c r="G35" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I35" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36">
-        <v>14.1</v>
+        <v>-0.8</v>
       </c>
       <c r="E36">
-        <v>-10.9</v>
+        <v>-3.3</v>
       </c>
       <c r="F36">
-        <v>46.1</v>
+        <v>1.7</v>
       </c>
       <c r="G36" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="I36" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>10.6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E37">
-        <v>-13.7</v>
+        <v>-3.4</v>
       </c>
       <c r="F37">
-        <v>41.8</v>
+        <v>21.1</v>
       </c>
       <c r="G37" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="I37" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -2330,27 +2288,27 @@
         <v>11</v>
       </c>
       <c r="D38">
-        <v>-7.2</v>
+        <v>-3.3</v>
       </c>
       <c r="E38">
-        <v>-10.9</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="F38">
-        <v>-3.4</v>
+        <v>-1.7</v>
       </c>
       <c r="G38" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="I38" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -2359,143 +2317,143 @@
         <v>11</v>
       </c>
       <c r="D39">
-        <v>27.9</v>
+        <v>-3.4</v>
       </c>
       <c r="E39">
-        <v>0.2</v>
+        <v>-11.8</v>
       </c>
       <c r="F39">
-        <v>63.2</v>
+        <v>5.8</v>
       </c>
       <c r="G39" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="I39" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D40">
-        <v>-7.2</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="E40">
-        <v>-11.7</v>
+        <v>-5.9</v>
       </c>
       <c r="F40">
-        <v>-2.6</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="G40" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="I40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
         <v>20</v>
       </c>
       <c r="D41">
-        <v>-7.2</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="E41">
-        <v>-11.9</v>
+        <v>-14.1</v>
       </c>
       <c r="F41">
-        <v>-2.4</v>
+        <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="I41" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42">
-        <v>4.5999999999999996</v>
+        <v>-2.4</v>
       </c>
       <c r="E42">
-        <v>-22.8</v>
+        <v>-4</v>
       </c>
       <c r="F42">
-        <v>41.7</v>
+        <v>-0.8</v>
       </c>
       <c r="G42" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="I42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
         <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D43">
-        <v>56.3</v>
+        <v>-4.5</v>
       </c>
       <c r="E43">
-        <v>6.4</v>
+        <v>-12.3</v>
       </c>
       <c r="F43">
-        <v>129.80000000000001</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G43" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="I43" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -2504,27 +2462,27 @@
         <v>11</v>
       </c>
       <c r="D44">
-        <v>-3.3</v>
+        <v>-7.2</v>
       </c>
       <c r="E44">
-        <v>-4.9000000000000004</v>
+        <v>-10.9</v>
       </c>
       <c r="F44">
-        <v>-1.7</v>
+        <v>-3.4</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H44" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="I44" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
@@ -2533,143 +2491,143 @@
         <v>11</v>
       </c>
       <c r="D45">
-        <v>-3.4</v>
+        <v>27.9</v>
       </c>
       <c r="E45">
-        <v>-11.8</v>
+        <v>0.2</v>
       </c>
       <c r="F45">
-        <v>5.8</v>
+        <v>63.2</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H45" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="I45" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D46">
+        <v>-7.2</v>
+      </c>
+      <c r="E46">
+        <v>-11.9</v>
+      </c>
+      <c r="F46">
         <v>-2.4</v>
       </c>
-      <c r="E46">
-        <v>-4</v>
-      </c>
-      <c r="F46">
-        <v>-0.8</v>
-      </c>
       <c r="G46" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H46" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
         <v>20</v>
       </c>
       <c r="D47">
-        <v>-4.0999999999999996</v>
+        <v>56.3</v>
       </c>
       <c r="E47">
-        <v>-5.9</v>
+        <v>6.4</v>
       </c>
       <c r="F47">
-        <v>-2.2999999999999998</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="G47" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H47" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I47" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
         <v>18</v>
       </c>
       <c r="D48">
-        <v>-4.5</v>
+        <v>-7.2</v>
       </c>
       <c r="E48">
-        <v>-12.3</v>
+        <v>-11.7</v>
       </c>
       <c r="F48">
-        <v>4.0999999999999996</v>
+        <v>-2.6</v>
       </c>
       <c r="G48" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H48" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="I48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D49">
-        <v>-2.2999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E49">
-        <v>-14.1</v>
+        <v>-22.8</v>
       </c>
       <c r="F49">
-        <v>11</v>
+        <v>41.7</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="H49" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I49" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -2678,27 +2636,27 @@
         <v>11</v>
       </c>
       <c r="D50">
-        <v>-6.9</v>
+        <v>-2.6</v>
       </c>
       <c r="E50">
-        <v>-9.1999999999999993</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="F50">
-        <v>-4.5</v>
+        <v>-0.5</v>
       </c>
       <c r="G50" t="s">
         <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="I50" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
         <v>15</v>
@@ -2707,147 +2665,150 @@
         <v>11</v>
       </c>
       <c r="D51">
-        <v>22.3</v>
+        <v>-11.6</v>
       </c>
       <c r="E51">
-        <v>0.8</v>
+        <v>-19</v>
       </c>
       <c r="F51">
-        <v>48.3</v>
+        <v>-3.6</v>
       </c>
       <c r="G51" t="s">
         <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="I51" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D52">
-        <v>-6.9</v>
+        <v>-2.5</v>
       </c>
       <c r="E52">
-        <v>-9.6999999999999993</v>
+        <v>-4.7</v>
       </c>
       <c r="F52">
-        <v>-4.0999999999999996</v>
+        <v>-0.3</v>
       </c>
       <c r="G52" t="s">
         <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="I52" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C53" t="s">
         <v>20</v>
       </c>
       <c r="D53">
-        <v>-6.8</v>
+        <v>-14.6</v>
       </c>
       <c r="E53">
-        <v>-9.5</v>
+        <v>-23.4</v>
       </c>
       <c r="F53">
-        <v>-4.0999999999999996</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="G53" t="s">
         <v>12</v>
       </c>
       <c r="H53" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="I53" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C54" t="s">
         <v>18</v>
       </c>
       <c r="D54">
-        <v>23.6</v>
+        <v>-2.6</v>
       </c>
       <c r="E54">
+        <v>-4.8</v>
+      </c>
+      <c r="F54">
+        <v>-0.5</v>
+      </c>
+      <c r="G54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55">
+        <v>-8.5</v>
+      </c>
+      <c r="E55">
+        <v>-16</v>
+      </c>
+      <c r="F55">
         <v>-0.3</v>
       </c>
-      <c r="F54">
-        <v>53.1</v>
-      </c>
-      <c r="G54" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" t="s">
-        <v>118</v>
-      </c>
-      <c r="I54" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" t="s">
-        <v>20</v>
-      </c>
-      <c r="D55">
-        <v>21</v>
-      </c>
-      <c r="E55">
-        <v>-10.199999999999999</v>
-      </c>
-      <c r="F55">
-        <v>62.9</v>
-      </c>
       <c r="G55" t="s">
         <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="I55" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C55" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:I55" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Hospital-associated"/>
+        <filter val="Acinetobacter Sp."/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I55">
+      <sortCondition ref="A1:A55"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2856,18 +2817,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I37"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2900,7 +2858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2929,7 +2887,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -2958,7 +2916,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -3016,7 +2974,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -3074,7 +3032,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3103,7 +3061,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -3132,7 +3090,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -3190,7 +3148,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -3248,7 +3206,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -3277,7 +3235,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -3306,7 +3264,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -3364,7 +3322,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -3422,7 +3380,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -3451,7 +3409,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -3480,7 +3438,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -3538,7 +3496,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -3592,11 +3550,11 @@
       <c r="H25" t="s">
         <v>166</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -3625,7 +3583,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -3654,7 +3612,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -3712,7 +3670,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>99</v>
       </c>
@@ -3770,7 +3728,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>110</v>
       </c>
@@ -3799,7 +3757,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>110</v>
       </c>
@@ -3828,7 +3786,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -3886,7 +3844,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -3945,13 +3903,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C37" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Hospital-associated"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -3963,13 +3914,14 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I37"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4012,24 +3964,6 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>7.3</v>
-      </c>
-      <c r="E2">
-        <v>0.2</v>
-      </c>
-      <c r="F2">
-        <v>14.9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I2" t="s">
-        <v>191</v>
-      </c>
     </row>
     <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4041,24 +3975,6 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>11.8</v>
-      </c>
-      <c r="E3">
-        <v>-24</v>
-      </c>
-      <c r="F3">
-        <v>64.5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" t="s">
-        <v>192</v>
-      </c>
-      <c r="I3" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -4070,26 +3986,8 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
-        <v>6.7</v>
-      </c>
-      <c r="E4">
-        <v>-2.4</v>
-      </c>
-      <c r="F4">
-        <v>16.8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" t="s">
-        <v>194</v>
-      </c>
-      <c r="I4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -4098,24 +3996,6 @@
       </c>
       <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="D5">
-        <v>7.9</v>
-      </c>
-      <c r="E5">
-        <v>-0.6</v>
-      </c>
-      <c r="F5">
-        <v>17.2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4128,26 +4008,8 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6">
-        <v>1.7</v>
-      </c>
-      <c r="E6">
-        <v>-43.4</v>
-      </c>
-      <c r="F6">
-        <v>82.8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" t="s">
-        <v>198</v>
-      </c>
-      <c r="I6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -4156,24 +4018,6 @@
       </c>
       <c r="C7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>-30.5</v>
-      </c>
-      <c r="F7">
-        <v>117.5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H7" t="s">
-        <v>200</v>
-      </c>
-      <c r="I7" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4199,7 +4043,7 @@
         <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="I8" t="s">
         <v>53</v>
@@ -4228,10 +4072,10 @@
         <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="I9" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4242,54 +4086,54 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>-2.6</v>
+        <v>2.4</v>
       </c>
       <c r="E10">
-        <v>-9.6999999999999993</v>
+        <v>-4.3</v>
       </c>
       <c r="F10">
-        <v>5.0999999999999996</v>
+        <v>9.6</v>
       </c>
       <c r="G10" t="s">
         <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="I10" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11">
-        <v>2.4</v>
+        <v>47.6</v>
       </c>
       <c r="E11">
-        <v>-4.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F11">
-        <v>9.6</v>
+        <v>108.6</v>
       </c>
       <c r="G11" t="s">
         <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="I11" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4297,31 +4141,31 @@
         <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>-10.5</v>
+        <v>-2.6</v>
       </c>
       <c r="E12">
-        <v>-32</v>
+        <v>-9.6999999999999993</v>
       </c>
       <c r="F12">
-        <v>17.899999999999999</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G12" t="s">
         <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="I12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -4329,25 +4173,25 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>47.6</v>
+        <v>-10.5</v>
       </c>
       <c r="E13">
-        <v>4.4000000000000004</v>
+        <v>-32</v>
       </c>
       <c r="F13">
-        <v>108.6</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="G13" t="s">
         <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="I13" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4373,10 +4217,10 @@
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="I14" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4402,10 +4246,10 @@
         <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="I15" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4416,54 +4260,54 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16">
-        <v>18.399999999999999</v>
+        <v>21.1</v>
       </c>
       <c r="E16">
-        <v>10.7</v>
+        <v>15</v>
       </c>
       <c r="F16">
-        <v>26.6</v>
+        <v>27.6</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="I16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
       <c r="D17">
-        <v>21.1</v>
+        <v>7.5</v>
       </c>
       <c r="E17">
-        <v>15</v>
+        <v>-19.8</v>
       </c>
       <c r="F17">
-        <v>27.6</v>
+        <v>44.2</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I17" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4471,31 +4315,31 @@
         <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18">
-        <v>4.4000000000000004</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="E18">
-        <v>-19.899999999999999</v>
+        <v>10.7</v>
       </c>
       <c r="F18">
-        <v>36.200000000000003</v>
+        <v>26.6</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="I18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -4503,25 +4347,25 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D19">
-        <v>7.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E19">
-        <v>-19.8</v>
+        <v>-19.899999999999999</v>
       </c>
       <c r="F19">
-        <v>44.2</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="I19" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4547,10 +4391,10 @@
         <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="I20" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4576,7 +4420,7 @@
         <v>76</v>
       </c>
       <c r="H21" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="I21" t="s">
         <v>44</v>
@@ -4590,54 +4434,54 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D22">
-        <v>15.9</v>
+        <v>24</v>
       </c>
       <c r="E22">
-        <v>3.3</v>
+        <v>11.1</v>
       </c>
       <c r="F22">
-        <v>29.9</v>
+        <v>38.4</v>
       </c>
       <c r="G22" t="s">
         <v>76</v>
       </c>
       <c r="H22" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="I22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23">
-        <v>24</v>
+        <v>-7.6</v>
       </c>
       <c r="E23">
-        <v>11.1</v>
+        <v>-49.5</v>
       </c>
       <c r="F23">
-        <v>38.4</v>
+        <v>69.2</v>
       </c>
       <c r="G23" t="s">
         <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="I23" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4645,31 +4489,31 @@
         <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24">
-        <v>-1.1000000000000001</v>
+        <v>15.9</v>
       </c>
       <c r="E24">
-        <v>-45.9</v>
+        <v>3.3</v>
       </c>
       <c r="F24">
-        <v>80.8</v>
+        <v>29.9</v>
       </c>
       <c r="G24" t="s">
         <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="I24" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -4677,25 +4521,25 @@
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>-7.6</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="E25">
-        <v>-49.5</v>
+        <v>-45.9</v>
       </c>
       <c r="F25">
-        <v>69.2</v>
+        <v>80.8</v>
       </c>
       <c r="G25" t="s">
         <v>76</v>
       </c>
       <c r="H25" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="I25" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4721,10 +4565,10 @@
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="I26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4750,10 +4594,10 @@
         <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="I27" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4764,54 +4608,54 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E28">
-        <v>-0.1</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="F28">
-        <v>6.2</v>
+        <v>3.4</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="I28" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="D29">
-        <v>0.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="E29">
-        <v>-2.2999999999999998</v>
+        <v>-3.6</v>
       </c>
       <c r="F29">
-        <v>3.4</v>
+        <v>25.9</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="I29" t="s">
-        <v>57</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4819,31 +4663,31 @@
         <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30">
-        <v>-0.2</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>-14.2</v>
+        <v>-0.1</v>
       </c>
       <c r="F30">
-        <v>16.100000000000001</v>
+        <v>6.2</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="I30" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -4851,28 +4695,28 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D31">
-        <v>10.199999999999999</v>
+        <v>-0.2</v>
       </c>
       <c r="E31">
-        <v>-3.6</v>
+        <v>-14.2</v>
       </c>
       <c r="F31">
-        <v>25.9</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="I31" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>110</v>
       </c>
@@ -4895,13 +4739,13 @@
         <v>76</v>
       </c>
       <c r="H32" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="I32" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>110</v>
       </c>
@@ -4924,13 +4768,13 @@
         <v>76</v>
       </c>
       <c r="H33" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="I33" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -4938,25 +4782,25 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D34">
-        <v>-3.9</v>
+        <v>-3.5</v>
       </c>
       <c r="E34">
-        <v>-9.5</v>
+        <v>-8.6</v>
       </c>
       <c r="F34">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="G34" t="s">
         <v>76</v>
       </c>
       <c r="H34" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="I34" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -4964,57 +4808,57 @@
         <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
         <v>20</v>
       </c>
       <c r="D35">
-        <v>-3.5</v>
+        <v>6</v>
       </c>
       <c r="E35">
-        <v>-8.6</v>
+        <v>-32.700000000000003</v>
       </c>
       <c r="F35">
-        <v>1.9</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="G35" t="s">
         <v>76</v>
       </c>
       <c r="H35" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="I35" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>110</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36">
-        <v>32.6</v>
+        <v>-3.9</v>
       </c>
       <c r="E36">
-        <v>-6.9</v>
+        <v>-9.5</v>
       </c>
       <c r="F36">
-        <v>88.7</v>
+        <v>2.1</v>
       </c>
       <c r="G36" t="s">
         <v>76</v>
       </c>
       <c r="H36" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="I36" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -5025,34 +4869,37 @@
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>32.6</v>
       </c>
       <c r="E37">
-        <v>-32.700000000000003</v>
+        <v>-6.9</v>
       </c>
       <c r="F37">
-        <v>66.900000000000006</v>
+        <v>88.7</v>
       </c>
       <c r="G37" t="s">
         <v>76</v>
       </c>
       <c r="H37" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="I37" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C37" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:I37" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Hospital-associated"/>
+        <filter val="Acinetobacter Sp."/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A32:I37">
+      <sortCondition descending="1" ref="C1:C37"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5061,11 +4908,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5105,7 +4951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -5128,13 +4974,13 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="I2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -5157,13 +5003,13 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="I3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -5171,25 +5017,25 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>-2.1</v>
+        <v>-0.9</v>
       </c>
       <c r="E4">
-        <v>-6.6</v>
+        <v>-5.3</v>
       </c>
       <c r="F4">
-        <v>2.7</v>
+        <v>3.6</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="I4" t="s">
-        <v>261</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5197,57 +5043,57 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5">
-        <v>-0.9</v>
+        <v>-6.1</v>
       </c>
       <c r="E5">
-        <v>-5.3</v>
+        <v>-29.7</v>
       </c>
       <c r="F5">
-        <v>3.6</v>
+        <v>25.4</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="I5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6">
-        <v>-16.3</v>
+        <v>-2.1</v>
       </c>
       <c r="E6">
-        <v>-32.5</v>
+        <v>-6.6</v>
       </c>
       <c r="F6">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="I6" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5258,28 +5104,28 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>-6.1</v>
+        <v>-16.3</v>
       </c>
       <c r="E7">
-        <v>-29.7</v>
+        <v>-32.5</v>
       </c>
       <c r="F7">
-        <v>25.4</v>
+        <v>3.8</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="I7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -5302,13 +5148,13 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="I8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -5331,13 +5177,13 @@
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="I9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -5345,25 +5191,25 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>-2</v>
+        <v>-0.5</v>
       </c>
       <c r="E10">
-        <v>-3.4</v>
+        <v>-1.7</v>
       </c>
       <c r="F10">
-        <v>-0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="I10" t="s">
-        <v>271</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5371,57 +5217,57 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11">
-        <v>-0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E11">
-        <v>-1.7</v>
+        <v>-6.4</v>
       </c>
       <c r="F11">
-        <v>0.7</v>
+        <v>7.2</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>0.2</v>
+        <v>-2</v>
       </c>
       <c r="E12">
-        <v>-7.1</v>
+        <v>-3.4</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>-0.5</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="I12" t="s">
-        <v>152</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5432,34 +5278,32 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>0.2</v>
       </c>
       <c r="E13">
-        <v>-6.4</v>
+        <v>-7.1</v>
       </c>
       <c r="F13">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="I13" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C13" xr:uid="{00000000-0001-0000-0300-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Hospital-associated"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:I13" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I13">
+      <sortCondition ref="A1:A13"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5468,11 +5312,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5480,6 +5323,7 @@
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -5511,7 +5355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -5534,13 +5378,13 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="I2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5563,13 +5407,13 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="I3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5592,10 +5436,10 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="I4" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5621,13 +5465,13 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="I5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -5650,7 +5494,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="I6" t="s">
         <v>59</v>
@@ -5679,20 +5523,13 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="I7" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C7" xr:uid="{00000000-0001-0000-0400-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Hospital-associated"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>